<commit_message>
added Sales order test case
</commit_message>
<xml_diff>
--- a/InputData/Customers_details.xlsx
+++ b/InputData/Customers_details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="104">
   <si>
     <t>Email</t>
   </si>
@@ -262,13 +262,79 @@
   </si>
   <si>
     <t>vTest 2020/02/14 12:56:43</t>
+  </si>
+  <si>
+    <t>Customer RFQ</t>
+  </si>
+  <si>
+    <t>REF number</t>
+  </si>
+  <si>
+    <t>GHT3453</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>HSN</t>
+  </si>
+  <si>
+    <t>Spcl.Dicsount</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>0020</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>Product2</t>
+  </si>
+  <si>
+    <t>TGS6768</t>
+  </si>
+  <si>
+    <t>34553</t>
+  </si>
+  <si>
+    <t>0050</t>
+  </si>
+  <si>
+    <t>0007</t>
+  </si>
+  <si>
+    <t>0012</t>
+  </si>
+  <si>
+    <t>00200</t>
+  </si>
+  <si>
+    <t>Internal remarks</t>
+  </si>
+  <si>
+    <t>Does not require constant supervision.</t>
+  </si>
+  <si>
+    <t>CustomerPO</t>
+  </si>
+  <si>
+    <t>TGTG6767</t>
+  </si>
+  <si>
+    <t>Expense</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +353,18 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF44435B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -316,7 +394,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -329,6 +407,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -624,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AU5"/>
+  <dimension ref="A1:AV11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -637,11 +724,16 @@
     <col min="3" max="3" width="24.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="8.7109375" style="1" collapsed="1"/>
-    <col min="8" max="8" width="9.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16" width="8.7109375" style="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" collapsed="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16" width="8.7109375" style="1" collapsed="1"/>
     <col min="17" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="8.7109375" style="1" collapsed="1"/>
+    <col min="18" max="47" width="8.7109375" style="1" collapsed="1"/>
+    <col min="48" max="48" width="8.7109375" style="1"/>
+    <col min="49" max="16384" width="8.7109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" s="4" customFormat="1" ht="45">
@@ -787,7 +879,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:47" ht="60">
+    <row r="2" spans="1:47" ht="30">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -894,7 +986,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="60">
+    <row r="3" spans="1:47" ht="30">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
@@ -1176,6 +1268,103 @@
       <c r="AU5" s="1">
         <v>46</v>
       </c>
+    </row>
+    <row r="7" spans="1:47" ht="30">
+      <c r="B7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" ht="78.75" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="6">
+        <v>57685</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47">
+      <c r="A9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="11" spans="1:47">
+      <c r="C11" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>